<commit_message>
removed files which are not part of the BA
</commit_message>
<xml_diff>
--- a/Collaborations/PFAS/Daten/Initials.xlsx
+++ b/Collaborations/PFAS/Daten/Initials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\OneDrive - bwedu\6. Semester\BA\Collaborations\PFAS\Daten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E88A68D-4B8A-43F2-A03C-25377E36EEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B7B44E-60B5-442D-8084-FF200DB52C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="777" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Experiment</t>
   </si>
@@ -216,7 +217,16 @@
     <t>total mass PFOS [µg/kg]</t>
   </si>
   <si>
-    <t>Total flux</t>
+    <t>exp. flux of N1_1</t>
+  </si>
+  <si>
+    <t>exp. flux of N1_3</t>
+  </si>
+  <si>
+    <t>used flux for N1_1</t>
+  </si>
+  <si>
+    <t>used flux for N1_3</t>
   </si>
 </sst>
 </file>
@@ -426,6 +436,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,12 +452,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -459,6 +469,1553 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Applied</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> Darcy fluxes in experiments</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hydraulics!$C$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exp. flux of N1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hydraulics!$B$7:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.8993000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7069000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.729200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.8979</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.7118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.738900000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.697900000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.713899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.698599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.723599999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40.747199999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44.720799999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.7194</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51.640999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>54.714599999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68.680599999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82.711799999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>96.970799999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>141.762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hydraulics!$F$7:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>49.494296000300189</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.449274111496763</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.848095388736056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.346723676259078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.12433757793784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.239479887318897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.8383915474869</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.235520562405164</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.998857234283204</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30.576460242037665</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.310402058729551</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.620731362842562</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36.235680894440648</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30.802669084518488</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.988280546701606</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.385848604924195</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.707012634505897</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31.266161033377518</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.75342805321727</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.16045285615774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-652A-465A-BF9C-E88ABE7B1E6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hydraulics!$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exp. flux of N1_3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hydraulics!$M$30:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.9333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.129899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.931899999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.957599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.5062</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.949300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107.908</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>146.91900000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159.173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hydraulics!$Q$30:$Q$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>23.929163137391242</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8129021055268213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.757420803507651</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2264596678674851</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3756334034321256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3207334510635782</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5913163324555857</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.84569364119554</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9447228573771795</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-652A-465A-BF9C-E88ABE7B1E6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hydraulics!$C$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>used flux for N1_3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hydraulics!$M$30:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.9333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.129899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.931899999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.957599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.5062</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.949300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107.908</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>146.91900000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159.173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hydraulics!$V$30:$V$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0458872800128933</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-652A-465A-BF9C-E88ABE7B1E6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hydraulics!$C$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>used flux for N1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="sq">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hydraulics!$B$7:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.8993000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7069000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.729200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.8979</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.7118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.738900000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.697900000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.713899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.698599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.723599999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40.747199999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44.720799999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.7194</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51.640999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>54.714599999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68.680599999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82.711799999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>96.970799999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>141.762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hydraulics!$K$7:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.675081468325722</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-652A-465A-BF9C-E88ABE7B1E6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="247583727"/>
+        <c:axId val="247591631"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="247583727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:t>t [d]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="247591631"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="247591631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:t>q</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600" baseline="0"/>
+                  <a:t> [cm/d]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="247583727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,6 +2062,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>465041</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>135589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>896469</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>156881</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E797157-FD37-9BD1-6ADD-25795E198C93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -775,27 +2368,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.3984375" customWidth="1"/>
-    <col min="6" max="6" width="14.1328125" customWidth="1"/>
-    <col min="7" max="7" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.86328125" customWidth="1"/>
-    <col min="10" max="10" width="7.86328125" customWidth="1"/>
-    <col min="11" max="11" width="14.73046875" customWidth="1"/>
-    <col min="12" max="12" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.46484375" customWidth="1"/>
-    <col min="37" max="37" width="12.265625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" customWidth="1"/>
+    <col min="37" max="37" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -860,7 +2454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -924,7 +2518,7 @@
         <v>34.835939343428329</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -988,7 +2582,7 @@
         <v>21.129995995194232</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1052,7 +2646,7 @@
         <v>10.279457511175574</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +2710,7 @@
         <v>34.835939343428329</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="AV6" s="27"/>
     </row>
   </sheetData>
@@ -1130,24 +2724,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AI142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.73046875" customWidth="1"/>
-    <col min="7" max="7" width="14.265625" customWidth="1"/>
-    <col min="8" max="9" width="16.3984375" customWidth="1"/>
-    <col min="10" max="10" width="11.265625" customWidth="1"/>
-    <col min="11" max="12" width="10.1328125" customWidth="1"/>
-    <col min="13" max="13" width="17.3984375" customWidth="1"/>
-    <col min="14" max="14" width="14.59765625" customWidth="1"/>
-    <col min="15" max="27" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="28" max="32" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="27" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1172,29 +2766,29 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="4" spans="1:35" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="43" t="s">
+    <row r="4" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="M4" s="43" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="M4" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
       <c r="X4" s="28"/>
       <c r="Y4" s="28"/>
       <c r="Z4" s="28"/>
@@ -1208,7 +2802,7 @@
       <c r="AH4" s="28"/>
       <c r="AI4" s="28"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1287,7 +2881,7 @@
       <c r="AH5" s="28"/>
       <c r="AI5" s="28"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1327,7 +2921,7 @@
       <c r="AH6" s="28"/>
       <c r="AI6" s="28"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>2.8993000000000002</v>
       </c>
@@ -1361,7 +2955,10 @@
         <f>I7+H7</f>
         <v>131.66773777087377</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="5">
+        <f>$E$52</f>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L7" s="5"/>
       <c r="M7" s="12">
         <v>1.9666999999999999</v>
@@ -1420,7 +3017,7 @@
       <c r="AH7" s="28"/>
       <c r="AI7" s="28"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>5.7069000000000001</v>
       </c>
@@ -1454,13 +3051,16 @@
         <f t="shared" ref="J8:J26" si="7">I8+H8</f>
         <v>128.08677117235024</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8:K26" si="8">$E$52</f>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="10">
         <v>8.7132000000000005</v>
       </c>
       <c r="N8" s="8">
-        <f t="shared" ref="N8:N16" si="8">M8-M7</f>
+        <f t="shared" ref="N8:N16" si="9">M8-M7</f>
         <v>6.7465000000000011</v>
       </c>
       <c r="O8" s="8">
@@ -1471,22 +3071,22 @@
         <v>0.52649521974357072</v>
       </c>
       <c r="Q8" s="10">
-        <f t="shared" ref="Q8:Q16" si="9">P8/$AC$7*1000</f>
+        <f t="shared" ref="Q8:Q16" si="10">P8/$AC$7*1000</f>
         <v>8.2759818998955978</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" ref="R8:R16" si="10">Q8/$Y$9*$AD$7</f>
+        <f t="shared" ref="R8:R16" si="11">Q8/$Y$9*$AD$7</f>
         <v>14.491783640933072</v>
       </c>
       <c r="S8" s="31">
-        <f t="shared" ref="S8:S16" si="11">R8-$AD$7</f>
+        <f t="shared" ref="S8:S16" si="12">R8-$AD$7</f>
         <v>-40.508216359066928</v>
       </c>
       <c r="T8" s="11">
         <v>148</v>
       </c>
       <c r="U8" s="31">
-        <f t="shared" ref="U8:U16" si="12">T8+S8</f>
+        <f t="shared" ref="U8:U16" si="13">T8+S8</f>
         <v>107.49178364093308</v>
       </c>
       <c r="X8" s="28" t="s">
@@ -1508,7 +3108,7 @@
       <c r="AH8" s="28"/>
       <c r="AI8" s="28"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>8.6999999999999993</v>
       </c>
@@ -1542,13 +3142,16 @@
         <f t="shared" si="7"/>
         <v>116.52767703917119</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L9" s="5"/>
       <c r="M9" s="10">
         <v>21.768799999999999</v>
       </c>
       <c r="N9" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13.055599999999998</v>
       </c>
       <c r="O9" s="8">
@@ -1559,22 +3162,22 @@
         <v>0.2814118079598027</v>
       </c>
       <c r="Q9" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.4235141018498538</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.7458614665932437</v>
       </c>
       <c r="S9" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-47.25413853340676</v>
       </c>
       <c r="T9" s="11">
         <v>148</v>
       </c>
       <c r="U9" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>100.74586146659324</v>
       </c>
       <c r="X9" s="28" t="s">
@@ -1595,7 +3198,7 @@
       <c r="AH9" s="28"/>
       <c r="AI9" s="28"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>12.729200000000001</v>
       </c>
@@ -1629,13 +3232,16 @@
         <f t="shared" si="7"/>
         <v>99.890155979460445</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="K10" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="10">
         <v>28.786799999999999</v>
       </c>
       <c r="N10" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.0180000000000007</v>
       </c>
       <c r="O10" s="8">
@@ -1646,22 +3252,22 @@
         <v>1.3016528925619832</v>
       </c>
       <c r="Q10" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.460690571960829</v>
       </c>
       <c r="R10" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>35.828002586215902</v>
       </c>
       <c r="S10" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-19.171997413784098</v>
       </c>
       <c r="T10" s="11">
         <v>148</v>
       </c>
       <c r="U10" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>128.82800258621592</v>
       </c>
       <c r="X10" s="28"/>
@@ -1677,7 +3283,7 @@
       <c r="AH10" s="28"/>
       <c r="AI10" s="28"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>15.8979</v>
       </c>
@@ -1711,13 +3317,16 @@
         <f t="shared" si="7"/>
         <v>95.998613091492658</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="K11" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L11" s="5"/>
       <c r="M11" s="10">
         <v>35.797199999999997</v>
       </c>
       <c r="N11" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.0103999999999971</v>
       </c>
       <c r="O11" s="8">
@@ -1728,22 +3337,22 @@
         <v>1.3391532580166614</v>
       </c>
       <c r="Q11" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21.050159068737578</v>
       </c>
       <c r="R11" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>36.860200338913074</v>
       </c>
       <c r="S11" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-18.139799661086926</v>
       </c>
       <c r="T11" s="11">
         <v>148</v>
       </c>
       <c r="U11" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>129.86020033891307</v>
       </c>
       <c r="X11" s="28"/>
@@ -1759,7 +3368,7 @@
       <c r="AH11" s="28"/>
       <c r="AI11" s="28"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
         <v>19.7118</v>
       </c>
@@ -1793,13 +3402,16 @@
         <f t="shared" si="7"/>
         <v>97.951299947490327</v>
       </c>
-      <c r="K12" s="5"/>
+      <c r="K12" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L12" s="5"/>
       <c r="M12" s="10">
         <v>43.794400000000003</v>
       </c>
       <c r="N12" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.9972000000000065</v>
       </c>
       <c r="O12" s="8">
@@ -1810,22 +3422,22 @@
         <v>1.310458660531185</v>
       </c>
       <c r="Q12" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.599108497888608</v>
       </c>
       <c r="R12" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>36.070381395018927</v>
       </c>
       <c r="S12" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-18.929618604981073</v>
       </c>
       <c r="T12" s="11">
         <v>148</v>
       </c>
       <c r="U12" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>129.07038139501893</v>
       </c>
       <c r="X12" s="28"/>
@@ -1841,7 +3453,7 @@
       <c r="AH12" s="28"/>
       <c r="AI12" s="28"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>22.738900000000001</v>
       </c>
@@ -1875,13 +3487,16 @@
         <f t="shared" si="7"/>
         <v>93.746837788860972</v>
       </c>
-      <c r="K13" s="5"/>
+      <c r="K13" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L13" s="5"/>
       <c r="M13" s="10">
         <v>63.772199999999998</v>
       </c>
       <c r="N13" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19.977799999999995</v>
       </c>
       <c r="O13" s="8">
@@ -1892,22 +3507,22 @@
         <v>1.3578572215158828</v>
       </c>
       <c r="Q13" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21.344166796768341</v>
       </c>
       <c r="R13" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>37.375027030769161</v>
       </c>
       <c r="S13" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-17.624972969230839</v>
       </c>
       <c r="T13" s="11">
         <v>148</v>
       </c>
       <c r="U13" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>130.37502703076916</v>
       </c>
       <c r="X13" s="28"/>
@@ -1923,7 +3538,7 @@
       <c r="AH13" s="28"/>
       <c r="AI13" s="28"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>26.697900000000001</v>
       </c>
@@ -1957,13 +3572,16 @@
         <f t="shared" si="7"/>
         <v>99.695432080150155</v>
       </c>
-      <c r="K14" s="5"/>
+      <c r="K14" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L14" s="5"/>
       <c r="M14" s="10">
         <v>89.685400000000001</v>
       </c>
       <c r="N14" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.913200000000003</v>
       </c>
       <c r="O14" s="8">
@@ -1974,22 +3592,22 @@
         <v>1.3275473503851318</v>
       </c>
       <c r="Q14" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.867725728626379</v>
       </c>
       <c r="R14" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>36.540747671451633</v>
       </c>
       <c r="S14" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-18.459252328548367</v>
       </c>
       <c r="T14" s="11">
         <v>148</v>
       </c>
       <c r="U14" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>129.54074767145164</v>
       </c>
       <c r="X14" s="28"/>
@@ -2005,7 +3623,7 @@
       <c r="AH14" s="28"/>
       <c r="AI14" s="28"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
         <v>29.713899999999999</v>
       </c>
@@ -2039,13 +3657,16 @@
         <f t="shared" si="7"/>
         <v>95.778888832374122</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L15" s="5"/>
       <c r="M15" s="10">
         <v>116.685</v>
       </c>
       <c r="N15" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26.999600000000001</v>
       </c>
       <c r="O15" s="8">
@@ -2056,22 +3677,22 @@
         <v>1.2815004666735803</v>
       </c>
       <c r="Q15" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.143914453893434</v>
       </c>
       <c r="R15" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>35.273306959621394</v>
       </c>
       <c r="S15" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-19.726693040378606</v>
       </c>
       <c r="T15" s="11">
         <v>148</v>
       </c>
       <c r="U15" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>128.27330695962138</v>
       </c>
       <c r="X15" s="28"/>
@@ -2087,7 +3708,7 @@
       <c r="AH15" s="28"/>
       <c r="AI15" s="28"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>33.698599999999999</v>
       </c>
@@ -2121,13 +3742,16 @@
         <f t="shared" si="7"/>
         <v>98.541374509143338</v>
       </c>
-      <c r="K16" s="5"/>
+      <c r="K16" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L16" s="5"/>
       <c r="M16" s="10">
         <v>159.93899999999999</v>
       </c>
       <c r="N16" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43.253999999999991</v>
       </c>
       <c r="O16" s="8">
@@ -2138,22 +3762,22 @@
         <v>1.439589402136219</v>
       </c>
       <c r="Q16" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.628915493598576</v>
       </c>
       <c r="R16" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>39.624705724202428</v>
       </c>
       <c r="S16" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-15.375294275797572</v>
       </c>
       <c r="T16" s="11">
         <v>148</v>
       </c>
       <c r="U16" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>132.62470572420244</v>
       </c>
       <c r="X16" s="28"/>
@@ -2169,7 +3793,7 @@
       <c r="AH16" s="28"/>
       <c r="AI16" s="28"/>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>36.723599999999998</v>
       </c>
@@ -2203,7 +3827,10 @@
         <f t="shared" si="7"/>
         <v>98.075489291529522</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="K17" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L17" s="5"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -2227,7 +3854,7 @@
       <c r="AH17" s="28"/>
       <c r="AI17" s="28"/>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>40.747199999999999</v>
       </c>
@@ -2261,7 +3888,10 @@
         <f t="shared" si="7"/>
         <v>98.618896126760021</v>
       </c>
-      <c r="K18" s="5"/>
+      <c r="K18" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L18" s="5"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
@@ -2285,7 +3915,7 @@
       <c r="AH18" s="28"/>
       <c r="AI18" s="28"/>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>44.720799999999997</v>
       </c>
@@ -2319,7 +3949,10 @@
         <f t="shared" si="7"/>
         <v>108.45103867503026</v>
       </c>
-      <c r="K19" s="5"/>
+      <c r="K19" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L19" s="5"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
@@ -2343,7 +3976,7 @@
       <c r="AH19" s="28"/>
       <c r="AI19" s="28"/>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
         <v>47.7194</v>
       </c>
@@ -2377,7 +4010,10 @@
         <f t="shared" si="7"/>
         <v>98.937480934042526</v>
       </c>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
@@ -2401,7 +4037,7 @@
       <c r="AH20" s="28"/>
       <c r="AI20" s="28"/>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
         <v>51.640999999999998</v>
       </c>
@@ -2435,7 +4071,10 @@
         <f t="shared" si="7"/>
         <v>99.262498700365697</v>
       </c>
-      <c r="K21" s="5"/>
+      <c r="K21" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L21" s="5"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
@@ -2459,7 +4098,7 @@
       <c r="AH21" s="28"/>
       <c r="AI21" s="28"/>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>54.714599999999997</v>
       </c>
@@ -2493,7 +4132,10 @@
         <f t="shared" si="7"/>
         <v>99.958666279270176</v>
       </c>
-      <c r="K22" s="5"/>
+      <c r="K22" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L22" s="5"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
@@ -2517,7 +4159,7 @@
       <c r="AH22" s="28"/>
       <c r="AI22" s="28"/>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>68.680599999999998</v>
       </c>
@@ -2551,7 +4193,10 @@
         <f t="shared" si="7"/>
         <v>100.52104542488033</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="K23" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L23" s="5"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
@@ -2575,7 +4220,7 @@
       <c r="AH23" s="28"/>
       <c r="AI23" s="28"/>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
         <v>82.711799999999997</v>
       </c>
@@ -2609,7 +4254,10 @@
         <f t="shared" si="7"/>
         <v>99.749085541619564</v>
       </c>
-      <c r="K24" s="5"/>
+      <c r="K24" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L24" s="5"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
@@ -2633,7 +4281,7 @@
       <c r="AH24" s="28"/>
       <c r="AI24" s="28"/>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
         <v>96.970799999999997</v>
       </c>
@@ -2667,7 +4315,10 @@
         <f t="shared" si="7"/>
         <v>98.851256679264651</v>
       </c>
-      <c r="K25" s="5"/>
+      <c r="K25" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L25" s="5"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
@@ -2691,7 +4342,7 @@
       <c r="AH25" s="28"/>
       <c r="AI25" s="28"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
         <v>141.762</v>
       </c>
@@ -2725,7 +4376,10 @@
         <f t="shared" si="7"/>
         <v>97.81291846584557</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="K26" s="5">
+        <f t="shared" si="8"/>
+        <v>31.675081468325722</v>
+      </c>
       <c r="L26" s="5"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
@@ -2749,24 +4403,24 @@
       <c r="AH26" s="28"/>
       <c r="AI26" s="28"/>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="2:35" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F28" s="13"/>
-      <c r="M28" s="45" t="s">
+      <c r="M28" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
-    </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.45">
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="48"/>
+      <c r="U28" s="48"/>
+    </row>
+    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="14">
         <f>Sheet1!L2*1000</f>
@@ -2799,7 +4453,7 @@
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="14">
         <f>C29/Sheet1!P2</f>
@@ -2824,7 +4478,7 @@
         <v>7.51</v>
       </c>
       <c r="P30" s="10">
-        <f t="shared" ref="P30:P38" si="13">O30/N30</f>
+        <f t="shared" ref="P30:P38" si="14">O30/N30</f>
         <v>1.5223075831593456</v>
       </c>
       <c r="Q30" s="10">
@@ -2846,8 +4500,12 @@
         <f>T30+S30</f>
         <v>129.90152408381169</v>
       </c>
-    </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.45">
+      <c r="V30">
+        <f>E53</f>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="14">
         <f>C30/Sheet1!U2</f>
@@ -2870,37 +4528,41 @@
         <v>13.129899999999999</v>
       </c>
       <c r="N31" s="10">
-        <f t="shared" ref="N31:N38" si="14">M31-M30</f>
+        <f t="shared" ref="N31:N38" si="15">M31-M30</f>
         <v>8.1966000000000001</v>
       </c>
       <c r="O31" s="10">
         <v>4.0739999999999998</v>
       </c>
       <c r="P31" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.4970353561232706</v>
       </c>
       <c r="Q31" s="10">
-        <f t="shared" ref="Q31:Q38" si="15">P31/$AC$7*1000</f>
+        <f t="shared" ref="Q31:Q38" si="16">P31/$AC$7*1000</f>
         <v>7.8129021055268213</v>
       </c>
       <c r="R31" s="10">
-        <f t="shared" ref="R31:R38" si="16">Q31/$Y$9*$AD$7</f>
+        <f t="shared" ref="R31:R38" si="17">Q31/$Y$9*$AD$7</f>
         <v>13.680900742727996</v>
       </c>
       <c r="S31" s="32">
-        <f t="shared" ref="S31:S38" si="17">R31-$AD$7</f>
+        <f t="shared" ref="S31:S38" si="18">R31-$AD$7</f>
         <v>-41.319099257272001</v>
       </c>
       <c r="T31" s="17">
         <v>143</v>
       </c>
       <c r="U31" s="32">
-        <f t="shared" ref="U31:U38" si="18">T31+S31</f>
+        <f t="shared" ref="U31:U38" si="19">T31+S31</f>
         <v>101.680900742728</v>
       </c>
-    </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.45">
+      <c r="V31">
+        <f>E53</f>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="14">
         <f>C31*52</f>
@@ -2916,37 +4578,41 @@
         <v>19.931899999999999</v>
       </c>
       <c r="N32" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.8019999999999996</v>
       </c>
       <c r="O32" s="10">
         <v>4.6550000000000002</v>
       </c>
       <c r="P32" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.68435754189944142</v>
       </c>
       <c r="Q32" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10.757420803507651</v>
       </c>
       <c r="R32" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>18.836944873075652</v>
       </c>
       <c r="S32" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-36.163055126924348</v>
       </c>
       <c r="T32" s="17">
         <v>143</v>
       </c>
       <c r="U32" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>106.83694487307565</v>
       </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="V32">
+        <f>$E$53</f>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -2964,37 +4630,41 @@
         <v>33.957599999999999</v>
       </c>
       <c r="N33" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14.025700000000001</v>
       </c>
       <c r="O33" s="10">
         <v>6.4480000000000004</v>
       </c>
       <c r="P33" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.45972750023171749</v>
       </c>
       <c r="Q33" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.2264596678674851</v>
       </c>
       <c r="R33" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12.654001816749474</v>
       </c>
       <c r="S33" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-42.345998183250529</v>
       </c>
       <c r="T33" s="17">
         <v>143</v>
       </c>
       <c r="U33" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>100.65400181674947</v>
       </c>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="V33">
+        <f t="shared" ref="V33:V38" si="20">$E$53</f>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -3007,44 +4677,43 @@
         <v>48.5062</v>
       </c>
       <c r="N34" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14.5486</v>
       </c>
       <c r="O34" s="10">
         <v>7.7519999999999998</v>
       </c>
       <c r="P34" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5328347744800187</v>
       </c>
       <c r="Q34" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.3756334034321256</v>
       </c>
       <c r="R34" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14.666279917775251</v>
       </c>
       <c r="S34" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-40.333720082224751</v>
       </c>
       <c r="T34" s="17">
         <v>143</v>
       </c>
       <c r="U34" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>102.66627991777526</v>
       </c>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B35" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="18">
-        <f>SUM(D6:D26)</f>
-        <v>285.66199999999998</v>
-      </c>
+      <c r="V34">
+        <f t="shared" si="20"/>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
       <c r="F35" s="19"/>
@@ -3060,142 +4729,162 @@
         <v>61.949300000000001</v>
       </c>
       <c r="N35" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>13.443100000000001</v>
       </c>
       <c r="O35" s="10">
         <v>7.1159999999999997</v>
       </c>
       <c r="P35" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.52934219041738872</v>
       </c>
       <c r="Q35" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.3207334510635782</v>
       </c>
       <c r="R35" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14.570146523424476</v>
       </c>
       <c r="S35" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-40.429853476575524</v>
       </c>
       <c r="T35" s="17">
         <v>143</v>
       </c>
       <c r="U35" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>102.57014652342448</v>
       </c>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="V35">
+        <f t="shared" si="20"/>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M36" s="10">
         <v>107.908</v>
       </c>
       <c r="N36" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>45.9587</v>
       </c>
       <c r="O36" s="10">
         <v>25.119</v>
       </c>
       <c r="P36" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5465559295628466</v>
       </c>
       <c r="Q36" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.5913163324555857</v>
       </c>
       <c r="R36" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15.04395478225147</v>
       </c>
       <c r="S36" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-39.956045217748532</v>
       </c>
       <c r="T36" s="17">
         <v>143</v>
       </c>
       <c r="U36" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>103.04395478225146</v>
       </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="V36">
+        <f t="shared" si="20"/>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M37" s="10">
         <v>146.91900000000001</v>
       </c>
       <c r="N37" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>39.01100000000001</v>
       </c>
       <c r="O37" s="10">
         <v>21.952999999999999</v>
       </c>
       <c r="P37" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.56273871472148862</v>
       </c>
       <c r="Q37" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.84569364119554</v>
       </c>
       <c r="R37" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15.489386027270109</v>
       </c>
       <c r="S37" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-39.510613972729892</v>
       </c>
       <c r="T37" s="17">
         <v>143</v>
       </c>
       <c r="U37" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>103.48938602727011</v>
       </c>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="V37">
+        <f t="shared" si="20"/>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M38" s="10">
         <v>159.173</v>
       </c>
       <c r="N38" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>12.253999999999991</v>
       </c>
       <c r="O38" s="10">
         <v>6.9729999999999999</v>
       </c>
       <c r="P38" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.56903868124694024</v>
       </c>
       <c r="Q38" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.9447228573771795</v>
       </c>
       <c r="R38" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15.662792638400278</v>
       </c>
       <c r="S38" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-39.337207361599724</v>
       </c>
       <c r="T38" s="17">
         <v>143</v>
       </c>
       <c r="U38" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>103.66279263840028</v>
       </c>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="V38">
+        <f t="shared" si="20"/>
+        <v>9.0458872800128933</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f>SUMPRODUCT(F7:F26,C7:C26)/B26</f>
+        <v>31.675081468325722</v>
+      </c>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
@@ -3206,7 +4895,7 @@
       <c r="T39" s="17"/>
       <c r="U39" s="32"/>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
@@ -3217,20 +4906,20 @@
       <c r="T40" s="17"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="43" spans="2:21" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="M43" s="45" t="s">
+    <row r="43" spans="2:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M43" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="N43" s="46"/>
-      <c r="O43" s="46"/>
-      <c r="P43" s="46"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="46"/>
-      <c r="S43" s="46"/>
-      <c r="T43" s="46"/>
-      <c r="U43" s="46"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
+      <c r="U43" s="48"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
@@ -3241,7 +4930,7 @@
       <c r="T44" s="10"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M45" s="10">
         <v>0.22220000000000001</v>
       </c>
@@ -3253,7 +4942,7 @@
         <v>0.82099999999999995</v>
       </c>
       <c r="P45" s="10">
-        <f t="shared" ref="P45:P55" si="19">O45/N45</f>
+        <f t="shared" ref="P45:P55" si="21">O45/N45</f>
         <v>3.6948694869486944</v>
       </c>
       <c r="Q45" s="10">
@@ -3276,357 +4965,377 @@
         <v>146.7013016992349</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M46" s="10">
         <v>0.85760000000000003</v>
       </c>
       <c r="N46" s="10">
-        <f t="shared" ref="N46:N55" si="20">M46-M45</f>
+        <f t="shared" ref="N46:N55" si="22">M46-M45</f>
         <v>0.63539999999999996</v>
       </c>
       <c r="O46" s="10">
         <v>3.0419999999999998</v>
       </c>
       <c r="P46" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.7875354107648729</v>
       </c>
       <c r="Q46" s="10">
-        <f t="shared" ref="Q46:Q55" si="21">P46/$AC$7*1000</f>
+        <f t="shared" ref="Q46:Q55" si="23">P46/$AC$7*1000</f>
         <v>75.255301318589346</v>
       </c>
       <c r="R46" s="10">
-        <f t="shared" ref="R46:R55" si="22">Q46/$Y$9*$AD$7</f>
+        <f t="shared" ref="R46:R55" si="24">Q46/$Y$9*$AD$7</f>
         <v>131.77693689204176</v>
       </c>
       <c r="S46" s="32">
-        <f t="shared" ref="S46:S55" si="23">R46-$AD$7</f>
+        <f t="shared" ref="S46:S55" si="25">R46-$AD$7</f>
         <v>76.776936892041761</v>
       </c>
       <c r="T46" s="17">
         <v>100</v>
       </c>
       <c r="U46" s="32">
-        <f t="shared" ref="U46:U55" si="24">T46+S46</f>
+        <f t="shared" ref="U46:U55" si="26">T46+S46</f>
         <v>176.77693689204176</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M47" s="10">
         <v>1.0693999999999999</v>
       </c>
       <c r="N47" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.21179999999999988</v>
       </c>
       <c r="O47" s="10">
         <v>0.98099999999999998</v>
       </c>
       <c r="P47" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.6317280453257821</v>
       </c>
       <c r="Q47" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>72.806164293428196</v>
       </c>
       <c r="R47" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>127.48833835413517</v>
       </c>
       <c r="S47" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>72.488338354135166</v>
       </c>
       <c r="T47" s="17">
         <v>100</v>
       </c>
       <c r="U47" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>172.48833835413518</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M48" s="10">
         <v>1.8575999999999999</v>
       </c>
       <c r="N48" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.78820000000000001</v>
       </c>
       <c r="O48" s="10">
         <v>3.3149999999999999</v>
       </c>
       <c r="P48" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.2057853336716571</v>
       </c>
       <c r="Q48" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>66.110767944418825</v>
       </c>
       <c r="R48" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>115.76426301736321</v>
       </c>
       <c r="S48" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>60.764263017363206</v>
       </c>
       <c r="T48" s="17">
         <v>100</v>
       </c>
       <c r="U48" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>160.76426301736319</v>
       </c>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
       <c r="M49" s="10">
         <v>3.0972</v>
       </c>
       <c r="N49" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.2396</v>
       </c>
       <c r="O49" s="10">
         <v>4.4790000000000001</v>
       </c>
       <c r="P49" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.6132623426911907</v>
       </c>
       <c r="Q49" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>56.796895064405419</v>
       </c>
       <c r="R49" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>99.455064632333972</v>
       </c>
       <c r="S49" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>44.455064632333972</v>
       </c>
       <c r="T49" s="17">
         <v>100</v>
       </c>
       <c r="U49" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>144.45506463233397</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
       <c r="M50" s="10">
         <v>5.9166999999999996</v>
       </c>
       <c r="N50" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.8194999999999997</v>
       </c>
       <c r="O50" s="10">
         <v>9.593</v>
       </c>
       <c r="P50" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.4023763078560032</v>
       </c>
       <c r="Q50" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>53.481976064596068</v>
       </c>
       <c r="R50" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>93.650425435012693</v>
       </c>
       <c r="S50" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>38.650425435012693</v>
       </c>
       <c r="T50" s="17">
         <v>100</v>
       </c>
       <c r="U50" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>138.65042543501269</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M51" s="10">
         <v>7.8958000000000004</v>
       </c>
       <c r="N51" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.9791000000000007</v>
       </c>
       <c r="O51" s="10">
         <v>5.9409999999999998</v>
       </c>
       <c r="P51" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.0018695366580759</v>
       </c>
       <c r="Q51" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>47.186407434677555</v>
       </c>
       <c r="R51" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>82.626474490584513</v>
       </c>
       <c r="S51" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>27.626474490584513</v>
       </c>
       <c r="T51" s="17">
         <v>100</v>
       </c>
       <c r="U51" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>127.62647449058451</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52">
+        <f>SUMPRODUCT(F7:F26,C7:C26)/B26</f>
+        <v>31.675081468325722</v>
+      </c>
       <c r="M52" s="10">
         <v>9.9319000000000006</v>
       </c>
       <c r="N52" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.0361000000000002</v>
       </c>
       <c r="O52" s="10">
         <v>6.1449999999999996</v>
       </c>
       <c r="P52" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.0180246549776526</v>
       </c>
       <c r="Q52" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>47.440349848188177</v>
       </c>
       <c r="R52" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>83.0711442057151</v>
       </c>
       <c r="S52" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.0711442057151</v>
       </c>
       <c r="T52" s="17">
         <v>100</v>
       </c>
       <c r="U52" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>128.07114420571509</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53">
+        <f>SUMPRODUCT(N30:N38,Q30:Q38)/M38</f>
+        <v>9.0458872800128933</v>
+      </c>
       <c r="M53" s="10">
         <v>12.934699999999999</v>
       </c>
       <c r="N53" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.0027999999999988</v>
       </c>
       <c r="O53" s="10">
         <v>9.7509999999999994</v>
       </c>
       <c r="P53" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.2473025176501942</v>
       </c>
       <c r="Q53" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>51.044370113460253</v>
       </c>
       <c r="R53" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>89.382018559188481</v>
       </c>
       <c r="S53" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>34.382018559188481</v>
       </c>
       <c r="T53" s="17">
         <v>100</v>
       </c>
       <c r="U53" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>134.38201855918848</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M54" s="10">
         <v>16.980599999999999</v>
       </c>
       <c r="N54" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>4.0458999999999996</v>
       </c>
       <c r="O54" s="10">
         <v>16.675999999999998</v>
       </c>
       <c r="P54" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.1217034528782222</v>
       </c>
       <c r="Q54" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>64.78908429476563</v>
       </c>
       <c r="R54" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>113.44990881453751</v>
       </c>
       <c r="S54" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>58.449908814537508</v>
       </c>
       <c r="T54" s="17">
         <v>100</v>
       </c>
       <c r="U54" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>158.44990881453751</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M55" s="10">
         <v>19.916699999999999</v>
       </c>
       <c r="N55" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.9360999999999997</v>
       </c>
       <c r="O55" s="10">
         <v>13.292999999999999</v>
       </c>
       <c r="P55" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.5274343516910189</v>
       </c>
       <c r="Q55" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>71.166771021795185</v>
       </c>
       <c r="R55" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>124.61765389852914</v>
       </c>
       <c r="S55" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>69.617653898529142</v>
       </c>
       <c r="T55" s="17">
         <v>100</v>
       </c>
       <c r="U55" s="32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>169.61765389852914</v>
       </c>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
@@ -3637,7 +5346,7 @@
       <c r="T56" s="17"/>
       <c r="U56" s="32"/>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
       <c r="O57" s="10"/>
@@ -3648,28 +5357,28 @@
       <c r="T57" s="17"/>
       <c r="U57" s="32"/>
     </row>
-    <row r="59" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="60" spans="2:21" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60" s="47"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
-      <c r="M60" s="47"/>
-      <c r="N60" s="48"/>
-      <c r="O60" s="48"/>
-      <c r="P60" s="48"/>
-      <c r="Q60" s="48"/>
-      <c r="R60" s="48"/>
-      <c r="S60" s="48"/>
-      <c r="T60" s="48"/>
-      <c r="U60" s="48"/>
-    </row>
-    <row r="61" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:21" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B60" s="43"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+      <c r="M60" s="43"/>
+      <c r="N60" s="44"/>
+      <c r="O60" s="44"/>
+      <c r="P60" s="44"/>
+      <c r="Q60" s="44"/>
+      <c r="R60" s="44"/>
+      <c r="S60" s="44"/>
+      <c r="T60" s="44"/>
+      <c r="U60" s="44"/>
+    </row>
+    <row r="61" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="35"/>
       <c r="C61" s="35"/>
       <c r="D61" s="35"/>
@@ -3689,7 +5398,7 @@
       <c r="T61" s="35"/>
       <c r="U61" s="35"/>
     </row>
-    <row r="62" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="36"/>
       <c r="C62" s="36"/>
       <c r="D62" s="36"/>
@@ -3709,7 +5418,7 @@
       <c r="T62" s="36"/>
       <c r="U62" s="36"/>
     </row>
-    <row r="63" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="37"/>
       <c r="C63" s="38"/>
       <c r="E63" s="39"/>
@@ -3726,7 +5435,7 @@
       <c r="T63" s="41"/>
       <c r="U63" s="41"/>
     </row>
-    <row r="64" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="37"/>
       <c r="C64" s="38"/>
       <c r="E64" s="39"/>
@@ -3743,7 +5452,7 @@
       <c r="T64" s="41"/>
       <c r="U64" s="41"/>
     </row>
-    <row r="65" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
       <c r="E65" s="39"/>
@@ -3760,7 +5469,7 @@
       <c r="T65" s="41"/>
       <c r="U65" s="41"/>
     </row>
-    <row r="66" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
       <c r="E66" s="39"/>
@@ -3777,7 +5486,7 @@
       <c r="T66" s="41"/>
       <c r="U66" s="41"/>
     </row>
-    <row r="67" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="E67" s="39"/>
@@ -3794,7 +5503,7 @@
       <c r="T67" s="41"/>
       <c r="U67" s="41"/>
     </row>
-    <row r="68" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="37"/>
       <c r="C68" s="38"/>
       <c r="E68" s="39"/>
@@ -3811,7 +5520,7 @@
       <c r="T68" s="41"/>
       <c r="U68" s="41"/>
     </row>
-    <row r="69" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="37"/>
       <c r="C69" s="38"/>
       <c r="E69" s="39"/>
@@ -3828,7 +5537,7 @@
       <c r="T69" s="41"/>
       <c r="U69" s="41"/>
     </row>
-    <row r="70" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="37"/>
       <c r="C70" s="38"/>
       <c r="E70" s="39"/>
@@ -3845,7 +5554,7 @@
       <c r="T70" s="41"/>
       <c r="U70" s="41"/>
     </row>
-    <row r="71" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="37"/>
       <c r="C71" s="38"/>
       <c r="E71" s="39"/>
@@ -3862,7 +5571,7 @@
       <c r="T71" s="41"/>
       <c r="U71" s="41"/>
     </row>
-    <row r="72" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="37"/>
       <c r="C72" s="38"/>
       <c r="E72" s="39"/>
@@ -3879,7 +5588,7 @@
       <c r="T72" s="41"/>
       <c r="U72" s="41"/>
     </row>
-    <row r="73" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="37"/>
       <c r="C73" s="38"/>
       <c r="E73" s="39"/>
@@ -3896,7 +5605,7 @@
       <c r="T73" s="41"/>
       <c r="U73" s="41"/>
     </row>
-    <row r="74" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="37"/>
       <c r="C74" s="38"/>
       <c r="E74" s="39"/>
@@ -3913,7 +5622,7 @@
       <c r="T74" s="41"/>
       <c r="U74" s="41"/>
     </row>
-    <row r="75" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="40"/>
       <c r="C75" s="40"/>
       <c r="D75" s="40"/>
@@ -3931,7 +5640,7 @@
       <c r="T75" s="41"/>
       <c r="U75" s="41"/>
     </row>
-    <row r="76" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="40"/>
       <c r="C76" s="40"/>
       <c r="D76" s="40"/>
@@ -3949,7 +5658,7 @@
       <c r="T76" s="41"/>
       <c r="U76" s="41"/>
     </row>
-    <row r="77" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="40"/>
       <c r="C77" s="40"/>
       <c r="D77" s="40"/>
@@ -3967,7 +5676,7 @@
       <c r="T77" s="41"/>
       <c r="U77" s="41"/>
     </row>
-    <row r="78" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="40"/>
       <c r="C78" s="40"/>
       <c r="D78" s="40"/>
@@ -3985,7 +5694,7 @@
       <c r="T78" s="41"/>
       <c r="U78" s="41"/>
     </row>
-    <row r="79" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="40"/>
       <c r="C79" s="40"/>
       <c r="D79" s="40"/>
@@ -4003,7 +5712,7 @@
       <c r="T79" s="41"/>
       <c r="U79" s="41"/>
     </row>
-    <row r="80" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="40"/>
       <c r="C80" s="40"/>
       <c r="D80" s="40"/>
@@ -4021,7 +5730,7 @@
       <c r="T80" s="41"/>
       <c r="U80" s="41"/>
     </row>
-    <row r="81" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="40"/>
       <c r="C81" s="40"/>
       <c r="D81" s="40"/>
@@ -4039,7 +5748,7 @@
       <c r="T81" s="41"/>
       <c r="U81" s="41"/>
     </row>
-    <row r="82" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="40"/>
       <c r="C82" s="40"/>
       <c r="D82" s="40"/>
@@ -4057,29 +5766,29 @@
       <c r="T82" s="41"/>
       <c r="U82" s="41"/>
     </row>
-    <row r="83" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="2:21" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B85" s="47"/>
-      <c r="C85" s="48"/>
-      <c r="D85" s="48"/>
-      <c r="E85" s="48"/>
-      <c r="F85" s="48"/>
-      <c r="G85" s="48"/>
-      <c r="H85" s="48"/>
-      <c r="I85" s="48"/>
-      <c r="J85" s="48"/>
-      <c r="M85" s="47"/>
-      <c r="N85" s="48"/>
-      <c r="O85" s="48"/>
-      <c r="P85" s="48"/>
-      <c r="Q85" s="48"/>
-      <c r="R85" s="48"/>
-      <c r="S85" s="48"/>
-      <c r="T85" s="48"/>
-      <c r="U85" s="48"/>
-    </row>
-    <row r="86" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:21" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B85" s="43"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="44"/>
+      <c r="J85" s="44"/>
+      <c r="M85" s="43"/>
+      <c r="N85" s="44"/>
+      <c r="O85" s="44"/>
+      <c r="P85" s="44"/>
+      <c r="Q85" s="44"/>
+      <c r="R85" s="44"/>
+      <c r="S85" s="44"/>
+      <c r="T85" s="44"/>
+      <c r="U85" s="44"/>
+    </row>
+    <row r="86" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="35"/>
       <c r="C86" s="35"/>
       <c r="D86" s="35"/>
@@ -4099,7 +5808,7 @@
       <c r="T86" s="35"/>
       <c r="U86" s="35"/>
     </row>
-    <row r="87" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="36"/>
       <c r="C87" s="36"/>
       <c r="D87" s="36"/>
@@ -4119,7 +5828,7 @@
       <c r="T87" s="36"/>
       <c r="U87" s="36"/>
     </row>
-    <row r="88" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C88" s="38"/>
       <c r="E88" s="39"/>
       <c r="G88" s="40"/>
@@ -4133,7 +5842,7 @@
       <c r="T88" s="41"/>
       <c r="U88" s="41"/>
     </row>
-    <row r="89" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C89" s="38"/>
       <c r="E89" s="39"/>
       <c r="G89" s="40"/>
@@ -4147,7 +5856,7 @@
       <c r="T89" s="41"/>
       <c r="U89" s="41"/>
     </row>
-    <row r="90" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C90" s="38"/>
       <c r="E90" s="39"/>
       <c r="G90" s="40"/>
@@ -4161,7 +5870,7 @@
       <c r="T90" s="41"/>
       <c r="U90" s="41"/>
     </row>
-    <row r="91" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C91" s="38"/>
       <c r="E91" s="39"/>
       <c r="G91" s="40"/>
@@ -4175,7 +5884,7 @@
       <c r="T91" s="41"/>
       <c r="U91" s="41"/>
     </row>
-    <row r="92" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C92" s="38"/>
       <c r="E92" s="39"/>
       <c r="G92" s="40"/>
@@ -4189,7 +5898,7 @@
       <c r="T92" s="41"/>
       <c r="U92" s="41"/>
     </row>
-    <row r="93" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C93" s="38"/>
       <c r="E93" s="39"/>
       <c r="G93" s="40"/>
@@ -4203,7 +5912,7 @@
       <c r="T93" s="41"/>
       <c r="U93" s="41"/>
     </row>
-    <row r="94" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C94" s="38"/>
       <c r="E94" s="39"/>
       <c r="G94" s="40"/>
@@ -4217,7 +5926,7 @@
       <c r="T94" s="41"/>
       <c r="U94" s="41"/>
     </row>
-    <row r="95" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C95" s="38"/>
       <c r="E95" s="39"/>
       <c r="G95" s="40"/>
@@ -4231,7 +5940,7 @@
       <c r="T95" s="41"/>
       <c r="U95" s="41"/>
     </row>
-    <row r="96" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C96" s="38"/>
       <c r="E96" s="39"/>
       <c r="G96" s="40"/>
@@ -4245,7 +5954,7 @@
       <c r="T96" s="41"/>
       <c r="U96" s="41"/>
     </row>
-    <row r="97" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C97" s="38"/>
       <c r="E97" s="39"/>
       <c r="G97" s="40"/>
@@ -4259,7 +5968,7 @@
       <c r="T97" s="41"/>
       <c r="U97" s="41"/>
     </row>
-    <row r="98" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C98" s="38"/>
       <c r="E98" s="39"/>
       <c r="G98" s="40"/>
@@ -4273,7 +5982,7 @@
       <c r="T98" s="41"/>
       <c r="U98" s="41"/>
     </row>
-    <row r="99" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C99" s="38"/>
       <c r="E99" s="39"/>
       <c r="G99" s="40"/>
@@ -4287,7 +5996,7 @@
       <c r="T99" s="41"/>
       <c r="U99" s="41"/>
     </row>
-    <row r="100" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C100" s="38"/>
       <c r="E100" s="39"/>
       <c r="G100" s="40"/>
@@ -4301,7 +6010,7 @@
       <c r="T100" s="41"/>
       <c r="U100" s="41"/>
     </row>
-    <row r="101" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C101" s="38"/>
       <c r="E101" s="39"/>
       <c r="G101" s="40"/>
@@ -4315,7 +6024,7 @@
       <c r="T101" s="41"/>
       <c r="U101" s="41"/>
     </row>
-    <row r="102" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C102" s="38"/>
       <c r="E102" s="39"/>
       <c r="G102" s="40"/>
@@ -4329,7 +6038,7 @@
       <c r="T102" s="41"/>
       <c r="U102" s="41"/>
     </row>
-    <row r="103" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C103" s="38"/>
       <c r="E103" s="39"/>
       <c r="G103" s="40"/>
@@ -4343,7 +6052,7 @@
       <c r="T103" s="41"/>
       <c r="U103" s="41"/>
     </row>
-    <row r="104" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C104" s="38"/>
       <c r="E104" s="39"/>
       <c r="G104" s="40"/>
@@ -4357,7 +6066,7 @@
       <c r="T104" s="41"/>
       <c r="U104" s="41"/>
     </row>
-    <row r="105" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C105" s="38"/>
       <c r="E105" s="39"/>
       <c r="G105" s="40"/>
@@ -4371,7 +6080,7 @@
       <c r="T105" s="41"/>
       <c r="U105" s="41"/>
     </row>
-    <row r="106" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C106" s="38"/>
       <c r="E106" s="39"/>
       <c r="G106" s="40"/>
@@ -4385,7 +6094,7 @@
       <c r="T106" s="41"/>
       <c r="U106" s="41"/>
     </row>
-    <row r="107" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C107" s="38"/>
       <c r="E107" s="39"/>
       <c r="G107" s="40"/>
@@ -4399,7 +6108,7 @@
       <c r="T107" s="41"/>
       <c r="U107" s="41"/>
     </row>
-    <row r="108" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C108" s="38"/>
       <c r="E108" s="39"/>
       <c r="G108" s="40"/>
@@ -4407,7 +6116,7 @@
       <c r="I108" s="41"/>
       <c r="J108" s="41"/>
     </row>
-    <row r="109" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C109" s="38"/>
       <c r="E109" s="39"/>
       <c r="G109" s="40"/>
@@ -4415,7 +6124,7 @@
       <c r="I109" s="41"/>
       <c r="J109" s="41"/>
     </row>
-    <row r="110" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C110" s="38"/>
       <c r="E110" s="39"/>
       <c r="G110" s="40"/>
@@ -4423,30 +6132,30 @@
       <c r="I110" s="41"/>
       <c r="J110" s="41"/>
     </row>
-    <row r="111" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="112" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="113" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="114" spans="2:32" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B114" s="47"/>
-      <c r="C114" s="48"/>
-      <c r="D114" s="48"/>
-      <c r="E114" s="48"/>
-      <c r="F114" s="48"/>
-      <c r="G114" s="48"/>
-      <c r="H114" s="48"/>
-      <c r="I114" s="48"/>
-      <c r="J114" s="48"/>
-      <c r="M114" s="47"/>
-      <c r="N114" s="48"/>
-      <c r="O114" s="48"/>
-      <c r="P114" s="48"/>
-      <c r="Q114" s="48"/>
-      <c r="R114" s="48"/>
-      <c r="S114" s="48"/>
-      <c r="T114" s="48"/>
-      <c r="U114" s="48"/>
-    </row>
-    <row r="115" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="3:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="2:32" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B114" s="43"/>
+      <c r="C114" s="44"/>
+      <c r="D114" s="44"/>
+      <c r="E114" s="44"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="44"/>
+      <c r="H114" s="44"/>
+      <c r="I114" s="44"/>
+      <c r="J114" s="44"/>
+      <c r="M114" s="43"/>
+      <c r="N114" s="44"/>
+      <c r="O114" s="44"/>
+      <c r="P114" s="44"/>
+      <c r="Q114" s="44"/>
+      <c r="R114" s="44"/>
+      <c r="S114" s="44"/>
+      <c r="T114" s="44"/>
+      <c r="U114" s="44"/>
+    </row>
+    <row r="115" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="35"/>
       <c r="C115" s="35"/>
       <c r="D115" s="35"/>
@@ -4466,7 +6175,7 @@
       <c r="T115" s="35"/>
       <c r="U115" s="35"/>
     </row>
-    <row r="116" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="36"/>
       <c r="C116" s="36"/>
       <c r="D116" s="36"/>
@@ -4486,7 +6195,7 @@
       <c r="T116" s="36"/>
       <c r="U116" s="36"/>
     </row>
-    <row r="117" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="37"/>
       <c r="C117" s="38"/>
       <c r="E117" s="39"/>
@@ -4502,7 +6211,7 @@
       <c r="T117" s="41"/>
       <c r="U117" s="41"/>
     </row>
-    <row r="118" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="37"/>
       <c r="C118" s="38"/>
       <c r="E118" s="39"/>
@@ -4518,7 +6227,7 @@
       <c r="T118" s="41"/>
       <c r="U118" s="41"/>
     </row>
-    <row r="119" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="37"/>
       <c r="C119" s="38"/>
       <c r="E119" s="39"/>
@@ -4545,7 +6254,7 @@
       <c r="AC119" s="42"/>
       <c r="AD119" s="42"/>
     </row>
-    <row r="120" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="37"/>
       <c r="C120" s="38"/>
       <c r="E120" s="39"/>
@@ -4574,7 +6283,7 @@
       <c r="AE120" s="42"/>
       <c r="AF120" s="42"/>
     </row>
-    <row r="121" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="37"/>
       <c r="C121" s="38"/>
       <c r="E121" s="39"/>
@@ -4590,7 +6299,7 @@
       <c r="T121" s="41"/>
       <c r="U121" s="41"/>
     </row>
-    <row r="122" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="37"/>
       <c r="C122" s="38"/>
       <c r="E122" s="39"/>
@@ -4606,7 +6315,7 @@
       <c r="T122" s="41"/>
       <c r="U122" s="41"/>
     </row>
-    <row r="123" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="37"/>
       <c r="C123" s="38"/>
       <c r="E123" s="39"/>
@@ -4622,7 +6331,7 @@
       <c r="T123" s="41"/>
       <c r="U123" s="41"/>
     </row>
-    <row r="124" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="37"/>
       <c r="C124" s="38"/>
       <c r="E124" s="39"/>
@@ -4638,7 +6347,7 @@
       <c r="T124" s="41"/>
       <c r="U124" s="41"/>
     </row>
-    <row r="125" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="37"/>
       <c r="C125" s="38"/>
       <c r="E125" s="39"/>
@@ -4654,7 +6363,7 @@
       <c r="T125" s="41"/>
       <c r="U125" s="41"/>
     </row>
-    <row r="126" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="37"/>
       <c r="C126" s="38"/>
       <c r="E126" s="39"/>
@@ -4670,7 +6379,7 @@
       <c r="T126" s="41"/>
       <c r="U126" s="41"/>
     </row>
-    <row r="127" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="37"/>
       <c r="C127" s="38"/>
       <c r="E127" s="39"/>
@@ -4685,29 +6394,29 @@
       <c r="T127" s="41"/>
       <c r="U127" s="41"/>
     </row>
-    <row r="128" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="129" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="130" spans="2:21" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B130" s="47"/>
-      <c r="C130" s="48"/>
-      <c r="D130" s="48"/>
-      <c r="E130" s="48"/>
-      <c r="F130" s="48"/>
-      <c r="G130" s="48"/>
-      <c r="H130" s="48"/>
-      <c r="I130" s="48"/>
-      <c r="J130" s="48"/>
-      <c r="M130" s="47"/>
-      <c r="N130" s="48"/>
-      <c r="O130" s="48"/>
-      <c r="P130" s="48"/>
-      <c r="Q130" s="48"/>
-      <c r="R130" s="48"/>
-      <c r="S130" s="48"/>
-      <c r="T130" s="48"/>
-      <c r="U130" s="48"/>
-    </row>
-    <row r="131" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:32" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:21" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B130" s="43"/>
+      <c r="C130" s="44"/>
+      <c r="D130" s="44"/>
+      <c r="E130" s="44"/>
+      <c r="F130" s="44"/>
+      <c r="G130" s="44"/>
+      <c r="H130" s="44"/>
+      <c r="I130" s="44"/>
+      <c r="J130" s="44"/>
+      <c r="M130" s="43"/>
+      <c r="N130" s="44"/>
+      <c r="O130" s="44"/>
+      <c r="P130" s="44"/>
+      <c r="Q130" s="44"/>
+      <c r="R130" s="44"/>
+      <c r="S130" s="44"/>
+      <c r="T130" s="44"/>
+      <c r="U130" s="44"/>
+    </row>
+    <row r="131" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="35"/>
       <c r="C131" s="35"/>
       <c r="D131" s="35"/>
@@ -4727,7 +6436,7 @@
       <c r="T131" s="35"/>
       <c r="U131" s="35"/>
     </row>
-    <row r="132" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="36"/>
       <c r="C132" s="36"/>
       <c r="D132" s="36"/>
@@ -4747,7 +6456,7 @@
       <c r="T132" s="36"/>
       <c r="U132" s="36"/>
     </row>
-    <row r="133" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="37"/>
       <c r="C133" s="38"/>
       <c r="E133" s="39"/>
@@ -4763,7 +6472,7 @@
       <c r="T133" s="41"/>
       <c r="U133" s="41"/>
     </row>
-    <row r="134" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="37"/>
       <c r="C134" s="38"/>
       <c r="E134" s="39"/>
@@ -4779,7 +6488,7 @@
       <c r="T134" s="41"/>
       <c r="U134" s="41"/>
     </row>
-    <row r="135" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="37"/>
       <c r="C135" s="38"/>
       <c r="E135" s="39"/>
@@ -4797,7 +6506,7 @@
       <c r="T135" s="41"/>
       <c r="U135" s="41"/>
     </row>
-    <row r="136" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="37"/>
       <c r="C136" s="38"/>
       <c r="E136" s="39"/>
@@ -4815,7 +6524,7 @@
       <c r="T136" s="41"/>
       <c r="U136" s="41"/>
     </row>
-    <row r="137" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="37"/>
       <c r="C137" s="38"/>
       <c r="E137" s="39"/>
@@ -4831,7 +6540,7 @@
       <c r="T137" s="41"/>
       <c r="U137" s="41"/>
     </row>
-    <row r="138" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="37"/>
       <c r="C138" s="38"/>
       <c r="E138" s="39"/>
@@ -4847,7 +6556,7 @@
       <c r="T138" s="41"/>
       <c r="U138" s="41"/>
     </row>
-    <row r="139" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="37"/>
       <c r="C139" s="38"/>
       <c r="E139" s="39"/>
@@ -4863,7 +6572,7 @@
       <c r="T139" s="41"/>
       <c r="U139" s="41"/>
     </row>
-    <row r="140" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B140" s="37"/>
       <c r="C140" s="38"/>
       <c r="E140" s="39"/>
@@ -4879,7 +6588,7 @@
       <c r="T140" s="41"/>
       <c r="U140" s="41"/>
     </row>
-    <row r="141" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="37"/>
       <c r="C141" s="38"/>
       <c r="E141" s="39"/>
@@ -4895,21 +6604,21 @@
       <c r="T141" s="41"/>
       <c r="U141" s="41"/>
     </row>
-    <row r="142" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="142" spans="2:21" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="M4:U4"/>
+    <mergeCell ref="M28:U28"/>
+    <mergeCell ref="M43:U43"/>
+    <mergeCell ref="M60:U60"/>
+    <mergeCell ref="B60:J60"/>
     <mergeCell ref="B114:J114"/>
     <mergeCell ref="M114:U114"/>
     <mergeCell ref="B130:J130"/>
     <mergeCell ref="M130:U130"/>
     <mergeCell ref="B85:J85"/>
     <mergeCell ref="M85:U85"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="M4:U4"/>
-    <mergeCell ref="M28:U28"/>
-    <mergeCell ref="M43:U43"/>
-    <mergeCell ref="M60:U60"/>
-    <mergeCell ref="B60:J60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4921,19 +6630,20 @@
   <dimension ref="B1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" customWidth="1"/>
-    <col min="11" max="13" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
@@ -4962,7 +6672,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -4999,7 +6709,7 @@
         <v>156.9</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -5036,7 +6746,7 @@
         <v>108.2</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -5073,7 +6783,7 @@
         <v>153.79999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>27</v>
       </c>

</xml_diff>